<commit_message>
🎡🔖 Checkpoint ./controllers/export_xlsx.js:1534710/276 ./controllers/exportcontroller.js:1534710/1819
</commit_message>
<xml_diff>
--- a/exports/registrations.xlsx
+++ b/exports/registrations.xlsx
@@ -29,7 +29,7 @@
       <name val="Verdana"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none">
         <fgColor rgb="FFFFFFFF"/>
@@ -38,12 +38,6 @@
     </fill>
     <fill>
       <patternFill patternType="lightGray"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00FF0000"/>
-        <bgColor rgb="FF000000"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -54,14 +48,8 @@
       <bottom style="none"/>
     </border>
   </borders>
-  <cellXfs count="3">
+  <cellXfs count="1">
     <xf applyAlignment="0" applyBorder="0" applyFont="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="0" numFmtId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="0" textRotation="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="1" applyFont="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="2" fontId="0" numFmtId="0">
-      <alignment horizontal="center" indent="0" shrinkToFit="0" textRotation="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="1" applyFont="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="0" numFmtId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="0" textRotation="0" vertical="bottom" wrapText="0"/>
     </xf>
   </cellXfs>
@@ -393,7 +381,7 @@
   <sheetPr filterMode="0">
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="1" rightToLeft="0" showFormulas="0" showGridLines="1" showOutlineSymbols="1" showRowColHeaders="1" showZeros="1" tabSelected="1" topLeftCell="A1" view="normal" windowProtection="0" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
       <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
@@ -402,26 +390,14 @@
   <sheetFormatPr defaultRowHeight="12.85"/>
   <cols>
     <col min="1" max="1" hidden="0" width="9.5" customWidth="0" collapsed="0" outlineLevel="0" style="0"/>
-    <col min="2" max="2" hidden="0" width="9.5" customWidth="0" collapsed="0" outlineLevel="0" style="0"/>
-    <col min="3" max="3" hidden="0" width="9.5" customWidth="0" collapsed="0" outlineLevel="0" style="0"/>
   </cols>
   <sheetData>
     <row r="1" outlineLevel="0">
-      <c r="A1" t="s" s="1">
+      <c r="A1" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="B1" t="s" s="2"/>
-      <c r="C1" t="s" s="2"/>
-    </row>
-    <row r="2" outlineLevel="0">
-      <c r="A2" t="s" s="2"/>
-      <c r="B2" t="s" s="2"/>
-      <c r="C2" t="s" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A1:C2"/>
-  </mergeCells>
   <printOptions gridLines="0" gridLinesSet="1" headings="0" horizontalCentered="0" verticalCentered="0"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup blackAndWhite="0" cellComments="none" copies="1" draft="0" firstPageNumber="1" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="1" usePrinterDefaults="0" verticalDpi="300"/>

</xml_diff>

<commit_message>
🍭🐷 Checkpoint ./controllers/exportcontroller.js:1534710/262 ./db.json:1534710/24
</commit_message>
<xml_diff>
--- a/exports/registrations.xlsx
+++ b/exports/registrations.xlsx
@@ -377,7 +377,7 @@
   <sheetPr filterMode="0">
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="1" rightToLeft="0" showFormulas="0" showGridLines="1" showOutlineSymbols="1" showRowColHeaders="1" showZeros="1" tabSelected="1" topLeftCell="A1" view="normal" windowProtection="0" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
       <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
@@ -387,15 +387,18 @@
   <cols>
     <col min="1" max="1" hidden="0" width="9.5" customWidth="0" collapsed="0" outlineLevel="0" style="0"/>
     <col min="2" max="2" hidden="0" width="9.5" customWidth="0" collapsed="0" outlineLevel="0" style="0"/>
+    <col min="3" max="3" hidden="0" width="9.5" customWidth="0" collapsed="0" outlineLevel="0" style="0"/>
   </cols>
   <sheetData>
     <row r="1" outlineLevel="0">
       <c r="A1" t="s" s="0"/>
       <c r="B1" t="s" s="0"/>
+      <c r="C1" t="s" s="0"/>
     </row>
     <row r="2" outlineLevel="0">
       <c r="A2" t="s" s="0"/>
       <c r="B2" t="s" s="0"/>
+      <c r="C2" t="s" s="0"/>
     </row>
   </sheetData>
   <printOptions gridLines="0" gridLinesSet="1" headings="0" horizontalCentered="0" verticalCentered="0"/>

</xml_diff>

<commit_message>
🍻🎏 Checkpoint ./controllers/exportcontroller.js:1534710/234 ./public/client.js:1534710/330
</commit_message>
<xml_diff>
--- a/exports/registrations.xlsx
+++ b/exports/registrations.xlsx
@@ -16,13 +16,22 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <si>
-    <t>title</t>
-  </si>
-  <si>
-    <t>guide</t>
-  </si>
-  <si>
-    <t>teamMembers</t>
+    <t>Project Title</t>
+  </si>
+  <si>
+    <t>Guide</t>
+  </si>
+  <si>
+    <t>USN1</t>
+  </si>
+  <si>
+    <t>USN2</t>
+  </si>
+  <si>
+    <t>USN3</t>
+  </si>
+  <si>
+    <t>USN4</t>
   </si>
   <si>
     <t>Killing Dumbledore 101</t>
@@ -31,8 +40,10 @@
     <t>Snape</t>
   </si>
   <si>
-    <t>1DS15IS061
-1DS15IS062</t>
+    <t>1DS15IS061</t>
+  </si>
+  <si>
+    <t>1DS15IS062</t>
   </si>
   <si>
     <t>Swish and Flick</t>
@@ -41,8 +52,10 @@
     <t>Flitwick</t>
   </si>
   <si>
-    <t>1DS15IS063
-1DS15IS064</t>
+    <t>1DS15IS063</t>
+  </si>
+  <si>
+    <t>1DS15IS064</t>
   </si>
   <si>
     <t>Transfiguration</t>
@@ -57,8 +70,34 @@
     <t>Defence Against The Dark Arts</t>
   </si>
   <si>
-    <t>1DS16IS003
-1DS16IS004</t>
+    <t>1DS16IS003</t>
+  </si>
+  <si>
+    <t>1DS16IS004</t>
+  </si>
+  <si>
+    <t>How to bring statues to life</t>
+  </si>
+  <si>
+    <t>1DS15IS033</t>
+  </si>
+  <si>
+    <t>1DS15IS044</t>
+  </si>
+  <si>
+    <t>It's Levi-oh-sah, not Levio-sah</t>
+  </si>
+  <si>
+    <t>Hermione</t>
+  </si>
+  <si>
+    <t>1DS16IS444</t>
+  </si>
+  <si>
+    <t>How to betray the most evil Wizard of all time while keeping a straight face</t>
+  </si>
+  <si>
+    <t>1DS16IS033</t>
   </si>
 </sst>
 </file>
@@ -423,7 +462,7 @@
   <sheetPr filterMode="0">
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="1" rightToLeft="0" showFormulas="0" showGridLines="1" showOutlineSymbols="1" showRowColHeaders="1" showZeros="1" tabSelected="1" topLeftCell="A1" view="normal" windowProtection="0" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
       <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
@@ -434,6 +473,9 @@
     <col min="1" max="1" hidden="0" width="9.5" customWidth="0" collapsed="0" outlineLevel="0" style="0"/>
     <col min="2" max="2" hidden="0" width="9.5" customWidth="0" collapsed="0" outlineLevel="0" style="0"/>
     <col min="3" max="3" hidden="0" width="9.5" customWidth="0" collapsed="0" outlineLevel="0" style="0"/>
+    <col min="4" max="4" hidden="0" width="9.5" customWidth="0" collapsed="0" outlineLevel="0" style="0"/>
+    <col min="5" max="5" hidden="0" width="9.5" customWidth="0" collapsed="0" outlineLevel="0" style="0"/>
+    <col min="6" max="6" hidden="0" width="9.5" customWidth="0" collapsed="0" outlineLevel="0" style="0"/>
   </cols>
   <sheetData>
     <row r="1" outlineLevel="0">
@@ -446,49 +488,103 @@
       <c r="C1" t="s" s="0">
         <v>2</v>
       </c>
+      <c r="D1" t="s" s="0">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s" s="0">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s" s="0">
+        <v>5</v>
+      </c>
     </row>
     <row r="2" outlineLevel="0">
       <c r="A2" t="s" s="0">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C2" t="s" s="0">
-        <v>5</v>
+        <v>8</v>
+      </c>
+      <c r="D2" t="s" s="0">
+        <v>9</v>
       </c>
     </row>
     <row r="3" outlineLevel="0">
       <c r="A3" t="s" s="0">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="C3" t="s" s="0">
-        <v>8</v>
+        <v>12</v>
+      </c>
+      <c r="D3" t="s" s="0">
+        <v>13</v>
       </c>
     </row>
     <row r="4" outlineLevel="0">
       <c r="A4" t="s" s="0">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="C4" t="s" s="0">
-        <v>11</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" outlineLevel="0">
       <c r="A5" t="s" s="0">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C5" t="s" s="0">
-        <v>13</v>
+        <v>18</v>
+      </c>
+      <c r="D5" t="s" s="0">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" outlineLevel="0">
+      <c r="A6" t="s" s="0">
+        <v>20</v>
+      </c>
+      <c r="B6" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="C6" t="s" s="0">
+        <v>21</v>
+      </c>
+      <c r="D6" t="s" s="0">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" outlineLevel="0">
+      <c r="A7" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="B7" t="s" s="0">
+        <v>24</v>
+      </c>
+      <c r="C7" t="s" s="0">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" outlineLevel="0">
+      <c r="A8" t="s" s="0">
+        <v>26</v>
+      </c>
+      <c r="B8" t="s" s="0">
+        <v>7</v>
+      </c>
+      <c r="C8" t="s" s="0">
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
📒🌃 Checkpoint ./controllers/socketcontroller.js:1534710/398 ./db.json:1534710/32916
</commit_message>
<xml_diff>
--- a/exports/registrations.xlsx
+++ b/exports/registrations.xlsx
@@ -28,6 +28,24 @@
     <t>Guide</t>
   </si>
   <si>
+    <t>Choice 1</t>
+  </si>
+  <si>
+    <t>Guide 1</t>
+  </si>
+  <si>
+    <t>Choice 2</t>
+  </si>
+  <si>
+    <t>Guide 2</t>
+  </si>
+  <si>
+    <t>Choice 3</t>
+  </si>
+  <si>
+    <t>Guide 3</t>
+  </si>
+  <si>
     <t>USN1</t>
   </si>
   <si>
@@ -40,16 +58,25 @@
     <t>USN4</t>
   </si>
   <si>
-    <t>9/3/2018, 6:15:00 AM</t>
-  </si>
-  <si>
-    <t>182.72.191.26,::ffff:10.10.11.196,::ffff:10.10.10.31</t>
-  </si>
-  <si>
-    <t>p1</t>
-  </si>
-  <si>
-    <t>A</t>
+    <t>9/3/2018, 6:12:45 PM</t>
+  </si>
+  <si>
+    <t>49.206.11.12,::ffff:10.10.10.247,::ffff:10.10.10.182</t>
+  </si>
+  <si>
+    <t>Blockchain in PDS and rural industries</t>
+  </si>
+  <si>
+    <t>Ms. SHARON CHRISTA I.L</t>
+  </si>
+  <si>
+    <t>Intelligent theft managment system using image processing technique</t>
+  </si>
+  <si>
+    <t>Mr. DHEEMANTH URS</t>
+  </si>
+  <si>
+    <t>Paperless tickets for indian transportation system</t>
   </si>
   <si>
     <t>1DS15IS001</t>
@@ -59,24 +86,6 @@
   </si>
   <si>
     <t>1DS15IS003</t>
-  </si>
-  <si>
-    <t>9/3/2018, 6:19:58 AM</t>
-  </si>
-  <si>
-    <t>182.72.191.26,::ffff:10.10.11.196,::ffff:10.10.10.231</t>
-  </si>
-  <si>
-    <t>p2</t>
-  </si>
-  <si>
-    <t>1DS15IS004</t>
-  </si>
-  <si>
-    <t>1DS15IS005</t>
-  </si>
-  <si>
-    <t>1DS15IS006</t>
   </si>
 </sst>
 </file>
@@ -441,7 +450,7 @@
   <sheetPr filterMode="0">
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="1" rightToLeft="0" showFormulas="0" showGridLines="1" showOutlineSymbols="1" showRowColHeaders="1" showZeros="1" tabSelected="1" topLeftCell="A1" view="normal" windowProtection="0" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
       <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
@@ -457,6 +466,12 @@
     <col min="6" max="6" hidden="0" width="9.5" customWidth="0" collapsed="0" outlineLevel="0" style="0"/>
     <col min="7" max="7" hidden="0" width="9.5" customWidth="0" collapsed="0" outlineLevel="0" style="0"/>
     <col min="8" max="8" hidden="0" width="9.5" customWidth="0" collapsed="0" outlineLevel="0" style="0"/>
+    <col min="9" max="9" hidden="0" width="9.5" customWidth="0" collapsed="0" outlineLevel="0" style="0"/>
+    <col min="10" max="10" hidden="0" width="9.5" customWidth="0" collapsed="0" outlineLevel="0" style="0"/>
+    <col min="11" max="11" hidden="0" width="9.5" customWidth="0" collapsed="0" outlineLevel="0" style="0"/>
+    <col min="12" max="12" hidden="0" width="9.5" customWidth="0" collapsed="0" outlineLevel="0" style="0"/>
+    <col min="13" max="13" hidden="0" width="9.5" customWidth="0" collapsed="0" outlineLevel="0" style="0"/>
+    <col min="14" max="14" hidden="0" width="9.5" customWidth="0" collapsed="0" outlineLevel="0" style="0"/>
   </cols>
   <sheetData>
     <row r="1" outlineLevel="0">
@@ -484,51 +499,64 @@
       <c r="H1" t="s" s="0">
         <v>7</v>
       </c>
+      <c r="I1" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="K1" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="L1" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="M1" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="N1" t="s" s="0">
+        <v>13</v>
+      </c>
     </row>
     <row r="2" outlineLevel="0">
       <c r="A2" t="s" s="0">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="C2" t="s" s="0">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="D2" t="s" s="0">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="E2" t="s" s="0">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="F2" t="s" s="0">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="G2" t="s" s="0">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="3" outlineLevel="0">
-      <c r="A3" t="s" s="0">
-        <v>15</v>
-      </c>
-      <c r="B3" t="s" s="0">
-        <v>16</v>
-      </c>
-      <c r="C3" t="s" s="0">
-        <v>17</v>
-      </c>
-      <c r="D3" t="s" s="0">
-        <v>11</v>
-      </c>
-      <c r="E3" t="s" s="0">
         <v>18</v>
       </c>
-      <c r="F3" t="s" s="0">
+      <c r="H2" t="s" s="0">
         <v>19</v>
       </c>
-      <c r="G3" t="s" s="0">
+      <c r="I2" t="s" s="0">
         <v>20</v>
+      </c>
+      <c r="J2" t="s" s="0">
+        <v>19</v>
+      </c>
+      <c r="K2" t="s" s="0">
+        <v>21</v>
+      </c>
+      <c r="L2" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="M2" t="s" s="0">
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
👆🏎 Checkpoint ./views/index.html:1534710/244 ./public/client.js:1534710/111 ./controllers/router.js:1534710/67
</commit_message>
<xml_diff>
--- a/exports/registrations.xlsx
+++ b/exports/registrations.xlsx
@@ -58,40 +58,40 @@
     <t>USN4</t>
   </si>
   <si>
-    <t>9/8/2018, 6:43:51 PM</t>
+    <t>9/9/2018, 5:58:55 AM</t>
   </si>
   <si>
     <t>nischal@nthacks.com</t>
   </si>
   <si>
-    <t>automatic street lighting using IOT</t>
-  </si>
-  <si>
-    <t>Ms. CHANDRAKALA B.M.</t>
-  </si>
-  <si>
-    <t>Blockchain in PDS and rural industries</t>
+    <t>Sound Regeneration using GAN's</t>
   </si>
   <si>
     <t>Ms. SHARON CHRISTA I.L</t>
   </si>
   <si>
-    <t>Advance Predictive Machine learning model using deep learning</t>
+    <t>Intelligent theft managment system using image processing technique</t>
+  </si>
+  <si>
+    <t>Mr. DHEEMANTH URS</t>
+  </si>
+  <si>
+    <t>3D model construction using multiple 2 D images</t>
   </si>
   <si>
     <t>Dr. SUNANDA DIXIT</t>
   </si>
   <si>
-    <t>1DS15IS907</t>
-  </si>
-  <si>
-    <t>1DS15IS919</t>
-  </si>
-  <si>
-    <t>1DS15IS922</t>
-  </si>
-  <si>
-    <t>1DS15IS925</t>
+    <t>1DS15IS801</t>
+  </si>
+  <si>
+    <t>1DS15IS802</t>
+  </si>
+  <si>
+    <t>1DS15IS803</t>
+  </si>
+  <si>
+    <t>1DS15IS804</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
👢🚌 Checkpoint ./db.json:1534710/41482:1565514/1 ./db1.json:1534710/1 ./server.js:1534710/42 ./public/client.js:1534710/402
</commit_message>
<xml_diff>
--- a/exports/registrations.xlsx
+++ b/exports/registrations.xlsx
@@ -58,40 +58,40 @@
     <t>USN4</t>
   </si>
   <si>
-    <t>9/9/2018, 5:58:55 AM</t>
-  </si>
-  <si>
-    <t>nischal@nthacks.com</t>
-  </si>
-  <si>
-    <t>Sound Regeneration using GAN's</t>
-  </si>
-  <si>
-    <t>Ms. SHARON CHRISTA I.L</t>
-  </si>
-  <si>
-    <t>Intelligent theft managment system using image processing technique</t>
-  </si>
-  <si>
-    <t>Mr. DHEEMANTH URS</t>
-  </si>
-  <si>
-    <t>3D model construction using multiple 2 D images</t>
-  </si>
-  <si>
-    <t>Dr. SUNANDA DIXIT</t>
-  </si>
-  <si>
-    <t>1DS15IS801</t>
-  </si>
-  <si>
-    <t>1DS15IS802</t>
-  </si>
-  <si>
-    <t>1DS15IS803</t>
-  </si>
-  <si>
-    <t>1DS15IS804</t>
+    <t>9/9/2018, 7:34:16 AM</t>
+  </si>
+  <si>
+    <t>svmasdhruthi@gmail.com</t>
+  </si>
+  <si>
+    <t>Chatbots in educational system</t>
+  </si>
+  <si>
+    <t>Ms. MADHURA J.</t>
+  </si>
+  <si>
+    <t>Detecting fraud apps using sentiment analysis</t>
+  </si>
+  <si>
+    <t>Mr. SURESHKUMAR M.</t>
+  </si>
+  <si>
+    <t>Web based library management system using angular and springboot</t>
+  </si>
+  <si>
+    <t>Ms. CHANDRAKALA B.M.</t>
+  </si>
+  <si>
+    <t>1DS15IS026</t>
+  </si>
+  <si>
+    <t>1DS15IS046</t>
+  </si>
+  <si>
+    <t>1DS15IS053</t>
+  </si>
+  <si>
+    <t>1DS15IS057</t>
   </si>
 </sst>
 </file>

</xml_diff>